<commit_message>
Note: Module 15 - add info from Forum
</commit_message>
<xml_diff>
--- a/LIRV/2019 S1/LIRV_Sem_1_2019_Q3_Appraisal_Value_Solutions_FINAL.xlsx
+++ b/LIRV/2019 S1/LIRV_Sem_1_2019_Q3_Appraisal_Value_Solutions_FINAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\EDUCATION\2019\Part III\Semester 1\Exams\Exam Questions and Solutions\LIRV\FINAL\Marking Guide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AACT196\Desktop\LIRV 2\Life Insurance and Retirement Valuation Exams 2019\LIRV Questions and Solutions_Semester 1 2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:8001_{F53E52BB-7A4D-405E-8D8F-334259956BB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA8678C-5099-47A3-AA00-1CCF27CCC7F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q3 Inputs" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
   <si>
     <t>Question 3</t>
   </si>
@@ -319,18 +319,22 @@
   <si>
     <t>Assets</t>
   </si>
+  <si>
+    <t>ANW + VEB (up to the 2019 sales tranche)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="0.0000000"/>
+  <numFmts count="5">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +383,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -415,10 +426,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -427,7 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -439,24 +451,26 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -470,6 +484,903 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q3c AV'!$K$26:$K$28</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>907668</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>949944.99600000028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3527410.1040000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FCDF-46D5-9E38-C01F11E9C94C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q3c AV'!$L$7:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3439020.8910000012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3330592.1579999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2862745.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FCDF-46D5-9E38-C01F11E9C94C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="389416272"/>
+        <c:axId val="488072208"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="389416272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488072208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="488072208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="389416272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>98425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>3175</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B52778BF-1FEA-43F9-8AC3-59027ACB684F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -771,26 +1682,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -798,7 +1709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -806,7 +1717,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -814,7 +1725,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -822,14 +1733,14 @@
         <v>43466</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="30.5" x14ac:dyDescent="0.5">
       <c r="A10" s="2"/>
       <c r="B10" s="7" t="s">
         <v>21</v>
@@ -838,7 +1749,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -846,7 +1757,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -854,7 +1765,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -865,7 +1776,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -876,7 +1787,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -887,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -895,12 +1806,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.5">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2016</v>
       </c>
@@ -908,7 +1819,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2017</v>
       </c>
@@ -916,7 +1827,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2018</v>
       </c>
@@ -924,7 +1835,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -932,7 +1843,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2020</v>
       </c>
@@ -940,7 +1851,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2021</v>
       </c>
@@ -958,32 +1869,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="6" width="10.42578125" customWidth="1"/>
+    <col min="2" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="6" width="10.453125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="15" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.7265625" customWidth="1"/>
+    <col min="9" max="15" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="16"/>
       <c r="B5" s="25" t="s">
         <v>37</v>
@@ -994,7 +1905,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -1032,7 +1943,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2019</v>
       </c>
@@ -1070,7 +1981,7 @@
         <f>H7*expenses</f>
         <v>777931.89000000013</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="6">
         <f>(G7+H7)*inv_rate</f>
         <v>523600.09500000003</v>
       </c>
@@ -1079,7 +1990,7 @@
         <v>2079463.8750000007</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2020</v>
       </c>
@@ -1126,7 +2037,7 @@
         <v>1657313.41875</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2021</v>
       </c>
@@ -1172,17 +2083,17 @@
         <v>1066979.7646875002</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>55</v>
       </c>
@@ -1200,40 +2111,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.26953125" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" customWidth="1"/>
+    <col min="14" max="14" width="15.26953125" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" customWidth="1"/>
+    <col min="16" max="16" width="12.26953125" customWidth="1"/>
+    <col min="17" max="17" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -1274,7 +2185,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <f>'Q3b Projected cash flows'!A7</f>
         <v>2019</v>
@@ -1310,7 +2221,7 @@
         <f>G7*inv_rate</f>
         <v>388965.94500000007</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="26">
         <f>H7+0.1*I7</f>
         <v>5523316.4189999998</v>
       </c>
@@ -1318,8 +2229,12 @@
         <f>G7+J7-H7-I7-(K8-K7)</f>
         <v>3439020.8910000012</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7" s="8">
+        <f>G7-H7-I7+J7</f>
+        <v>1944829.7250000008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <f>'Q3b Projected cash flows'!A8</f>
         <v>2020</v>
@@ -1355,7 +2270,7 @@
         <f>G8*inv_rate</f>
         <v>283741.21500000003</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="26">
         <f t="shared" ref="K8:K9" si="0">H8+0.1*I8</f>
         <v>4029125.2529999996</v>
       </c>
@@ -1364,9 +2279,12 @@
         <v>3330592.1579999994</v>
       </c>
       <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="8">
+        <f t="shared" ref="N8:N9" si="2">G8-H8-I8+J8</f>
+        <v>1418706.075</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <f>'Q3b Projected cash flows'!A9</f>
         <v>2021</v>
@@ -1402,7 +2320,7 @@
         <f>G9*inv_rate</f>
         <v>149101.35</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="26">
         <f t="shared" si="0"/>
         <v>2117239.17</v>
       </c>
@@ -1411,16 +2329,19 @@
         <v>2862745.92</v>
       </c>
       <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N9" s="8">
+        <f t="shared" si="2"/>
+        <v>745506.75000000012</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L11" s="6">
         <f>NPV(hurdle,L7:L9)</f>
         <v>8029761.5115777599</v>
       </c>
       <c r="N11" s="14"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1432,7 +2353,7 @@
         <v>25000000</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>60</v>
@@ -1441,7 +2362,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>61</v>
       </c>
@@ -1450,7 +2371,7 @@
         <v>7779318.9000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>62</v>
       </c>
@@ -1459,7 +2380,7 @@
         <v>5523316.4189999998</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>44</v>
       </c>
@@ -1468,24 +2389,24 @@
         <v>10697364.681</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="D18" s="13"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
         <v>64</v>
       </c>
@@ -1500,7 +2421,7 @@
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
     </row>
-    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>15</v>
       </c>
@@ -1535,7 +2456,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2020</v>
       </c>
@@ -1579,7 +2500,7 @@
       </c>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2021</v>
       </c>
@@ -1608,23 +2529,23 @@
         <v>224460</v>
       </c>
       <c r="H27" s="6">
-        <f t="shared" ref="H27:H28" si="2">SUM(C27:D27)-SUM(E27:F27)+G27</f>
+        <f t="shared" ref="H27:H28" si="3">SUM(C27:D27)-SUM(E27:F27)+G27</f>
         <v>1842300</v>
       </c>
       <c r="I27" s="6">
-        <f t="shared" ref="I27:I28" si="3">D27-E27-F27+G27</f>
+        <f t="shared" ref="I27:I28" si="4">D27-E27-F27+G27</f>
         <v>942300</v>
       </c>
       <c r="J27" s="6">
-        <f t="shared" ref="J27:J28" si="4">E27+0.1*F27</f>
+        <f t="shared" ref="J27:J28" si="5">E27+0.1*F27</f>
         <v>2548332</v>
       </c>
       <c r="K27" s="6">
-        <f t="shared" ref="K27:K28" si="5">I27-(J28-J27)</f>
+        <f t="shared" ref="K27:K28" si="6">I27-(J28-J27)</f>
         <v>949944.99600000028</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2022</v>
       </c>
@@ -1653,23 +2574,23 @@
         <v>271036.62000000005</v>
       </c>
       <c r="H28" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2829023.1000000006</v>
       </c>
       <c r="I28" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>986723.10000000033</v>
       </c>
       <c r="J28" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2540687.0039999997</v>
       </c>
       <c r="K28" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3527410.1040000003</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B29" s="8"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -1679,7 +2600,7 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B30" s="8"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -1694,7 +2615,7 @@
       </c>
       <c r="L30" s="12"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1703,7 +2624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -1712,7 +2633,7 @@
         <v>17044266.563486103</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -1720,8 +2641,11 @@
         <f>D16+L11</f>
         <v>18727126.192577761</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1730,7 +2654,7 @@
         <v>17044266.563486103</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -1745,6 +2669,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1753,22 +2678,22 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1779,7 +2704,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1790,7 +2715,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1801,7 +2726,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1810,7 +2735,7 @@
       </c>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1819,12 +2744,12 @@
       </c>
       <c r="D8" s="18"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -1833,7 +2758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -1842,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -1851,7 +2776,7 @@
         <v>5445523.2299999995</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -1860,20 +2785,20 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>15</v>
       </c>
@@ -1890,7 +2815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1899,7 +2824,7 @@
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <f>1+A22</f>
         <v>2020</v>
@@ -1909,7 +2834,7 @@
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <f>1+A23</f>
         <v>2021</v>
@@ -1919,12 +2844,12 @@
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
@@ -1941,7 +2866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2019</v>
       </c>
@@ -1950,7 +2875,7 @@
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <f>1+A30</f>
         <v>2020</v>
@@ -1960,7 +2885,7 @@
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <f>1+A31</f>
         <v>2021</v>
@@ -1970,12 +2895,12 @@
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>15</v>
       </c>
@@ -1992,7 +2917,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2019</v>
       </c>
@@ -2001,7 +2926,7 @@
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <f>1+A38</f>
         <v>2020</v>
@@ -2011,7 +2936,7 @@
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <f>1+A39</f>
         <v>2021</v>
@@ -2021,7 +2946,7 @@
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -2029,7 +2954,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>15</v>
       </c>
@@ -2046,7 +2971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2019</v>
       </c>
@@ -2055,7 +2980,7 @@
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <f>1+A45</f>
         <v>2020</v>
@@ -2065,7 +2990,7 @@
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <f>1+A46</f>
         <v>2021</v>
@@ -2075,12 +3000,12 @@
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>15</v>
       </c>
@@ -2097,7 +3022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2019</v>
       </c>
@@ -2106,7 +3031,7 @@
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53">
         <f>1+A52</f>
         <v>2020</v>
@@ -2116,7 +3041,7 @@
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54">
         <f>1+A53</f>
         <v>2021</v>

</xml_diff>